<commit_message>
added upload changed files, zip doesnt work, corrected layout of stuff on sheets
</commit_message>
<xml_diff>
--- a/IndPlanExample.xlsx
+++ b/IndPlanExample.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <fileSharing userName="DDDD" algorithmName="SHA-512" hashValue="BjE+G6cAgUqCtEo7t0HGr3AgFs/yLBdTxnDgfmJkzte7Bk3JqlCq9Qt5q8HutxsI+LUYk4gcPaYQ/KSI2TnzgA==" saltValue="KhAm0W4atNJhXI/MaCQvpQ==" spinCount="100000"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Trash\IntelliJ IDEA 2020.3.2\workspace\SLDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF00DE6E-EC2C-428D-A25A-A2F73466D820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B80D69-F6B2-43D2-8FA8-D56BCBA1247F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="926" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="926" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТИТУЛ" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="122">
   <si>
     <t>МІНІСТЕРСТВО ОСВІТИ І НАУКИ УКРАЇНИ                                                                                                                     НАЦІОНАЛЬНИЙ ТЕХНІЧНИЙ УНІВЕРСИТЕТ 
 "ХАРКІВСЬКИЙ ПОЛІТЕХНІЧНИЙ ІНСТИТУТ"</t>
@@ -891,9 +890,6 @@
     <t>Викладач 14</t>
   </si>
   <si>
-    <t>План розглянуто на засіданні кафедри "___" ________ 20__р. Протокол № ___</t>
-  </si>
-  <si>
     <t xml:space="preserve">Індивідуальний план склав _______________ </t>
   </si>
   <si>
@@ -1014,6 +1010,18 @@
       </rPr>
       <t xml:space="preserve"> р.</t>
     </r>
+  </si>
+  <si>
+    <t>Протокол</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" 30 " серпня 2021 р. </t>
+  </si>
+  <si>
+    <t>Протокол № 1</t>
+  </si>
+  <si>
+    <t>(підпис)</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2083,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="250">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2523,6 +2531,59 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2540,45 +2601,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2606,66 +2649,114 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2674,72 +2765,6 @@
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2781,10 +2806,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2813,6 +2834,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3193,7 +3218,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="69" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3345,10 +3370,10 @@
         <v>#N/A</v>
       </c>
       <c r="K8" s="35"/>
-      <c r="L8" s="161" t="s">
+      <c r="L8" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="162" t="s">
+      <c r="M8" s="173" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3364,8 +3389,8 @@
       <c r="E9" s="170"/>
       <c r="F9" s="170"/>
       <c r="G9" s="48"/>
-      <c r="L9" s="161"/>
-      <c r="M9" s="162"/>
+      <c r="L9" s="172"/>
+      <c r="M9" s="173"/>
       <c r="N9" s="36"/>
     </row>
     <row r="10" spans="1:14" ht="5.25" customHeight="1">
@@ -3402,17 +3427,17 @@
       <c r="E12" s="171"/>
       <c r="F12" s="171"/>
       <c r="G12" s="47"/>
-      <c r="L12" s="163" t="s">
+      <c r="L12" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="162" t="s">
+      <c r="M12" s="173" t="s">
         <v>6</v>
       </c>
       <c r="N12" s="36"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="L13" s="163"/>
-      <c r="M13" s="162"/>
+      <c r="L13" s="174"/>
+      <c r="M13" s="173"/>
       <c r="N13" s="36"/>
     </row>
     <row r="14" spans="1:14">
@@ -3512,10 +3537,10 @@
       <c r="E24" s="168"/>
       <c r="F24" s="168"/>
       <c r="G24" s="168"/>
-      <c r="L24" s="163" t="s">
+      <c r="L24" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="M24" s="162" t="s">
+      <c r="M24" s="173" t="s">
         <v>13</v>
       </c>
       <c r="N24" s="36"/>
@@ -3530,8 +3555,8 @@
       <c r="E25" s="164"/>
       <c r="F25" s="164"/>
       <c r="G25" s="164"/>
-      <c r="L25" s="163"/>
-      <c r="M25" s="162"/>
+      <c r="L25" s="174"/>
+      <c r="M25" s="173"/>
       <c r="N25" s="36"/>
     </row>
     <row r="26" spans="1:14">
@@ -3620,10 +3645,10 @@
       <c r="E33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="157" t="s">
+      <c r="F33" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="158"/>
+      <c r="G33" s="178"/>
       <c r="M33" s="54"/>
       <c r="N33" s="36"/>
     </row>
@@ -3643,52 +3668,93 @@
       <c r="E34" s="93">
         <v>1.5</v>
       </c>
-      <c r="F34" s="159" t="s">
+      <c r="F34" s="179" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="160"/>
-      <c r="L34" s="163" t="s">
+      <c r="G34" s="180"/>
+      <c r="L34" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="M34" s="162" t="s">
+      <c r="M34" s="173" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="L35" s="163"/>
-      <c r="M35" s="162"/>
+      <c r="L35" s="174"/>
+      <c r="M35" s="173"/>
     </row>
     <row r="36" spans="1:14" ht="18.75">
       <c r="B36" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="M36" s="156" t="s">
+      <c r="C36" s="161" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="160"/>
+      <c r="E36" s="160"/>
+      <c r="M36" s="176" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="18.75">
       <c r="B37" s="131" t="s">
-        <v>118</v>
-      </c>
-      <c r="M37" s="156"/>
+        <v>117</v>
+      </c>
+      <c r="C37" s="175" t="str">
+        <f>'СПИСКИ (пароль 123)'!J2</f>
+        <v xml:space="preserve">" 30 " серпня 2021 р. </v>
+      </c>
+      <c r="D37" s="175"/>
+      <c r="E37" s="175"/>
+      <c r="M37" s="176"/>
     </row>
     <row r="38" spans="1:14" ht="18.75">
       <c r="B38" s="131" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" ht="18.75">
+      <c r="C38" s="175" t="str">
+        <f>'СПИСКИ (пароль 123)'!J3</f>
+        <v>Протокол № 1</v>
+      </c>
+      <c r="D38" s="175"/>
+      <c r="E38" s="175"/>
+    </row>
+    <row r="39" spans="1:14" ht="20.25">
       <c r="B39" s="131" t="s">
         <v>28</v>
       </c>
+      <c r="C39" s="162" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="160"/>
+      <c r="E39" s="160"/>
     </row>
     <row r="40" spans="1:14">
       <c r="B40" s="132" t="s">
         <v>29</v>
       </c>
+      <c r="C40" s="160"/>
+      <c r="D40" s="163" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" s="160"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A20:G20"/>
@@ -3696,18 +3762,6 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="A25:G25"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="4">
@@ -3765,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E42544-BB4C-415B-B5D9-3929201D8D8D}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3782,44 +3836,44 @@
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
     </row>
     <row r="2" spans="1:5" ht="58.5" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
-      <c r="B3" s="172"/>
-      <c r="C3" s="172"/>
-      <c r="D3" s="172"/>
-      <c r="E3" s="172"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
     </row>
     <row r="4" spans="1:5" ht="66" customHeight="1">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="172"/>
-      <c r="B5" s="172"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
+      <c r="A5" s="181"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="172"/>
-      <c r="B6" s="172"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
+      <c r="A6" s="181"/>
+      <c r="B6" s="181"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
@@ -3836,27 +3890,27 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="172"/>
-      <c r="B9" s="172"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
+      <c r="A9" s="181"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="172"/>
-      <c r="B10" s="172"/>
-      <c r="C10" s="172"/>
-      <c r="D10" s="172"/>
-      <c r="E10" s="172"/>
+      <c r="A10" s="181"/>
+      <c r="B10" s="181"/>
+      <c r="C10" s="181"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1">
       <c r="A11" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="172"/>
-      <c r="C11" s="172"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="172"/>
+      <c r="B11" s="181"/>
+      <c r="C11" s="181"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
     </row>
     <row r="12" spans="1:5" ht="21" customHeight="1" thickBot="1">
       <c r="A12" s="149"/>
@@ -3888,47 +3942,47 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1">
-      <c r="A15" s="174" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="174"/>
-      <c r="C15" s="174"/>
+      <c r="A15" s="189" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="189"/>
+      <c r="C15" s="189"/>
       <c r="D15" s="150"/>
       <c r="E15" s="151"/>
     </row>
     <row r="16" spans="1:5" ht="33" customHeight="1">
-      <c r="A16" s="175" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="176"/>
-      <c r="C16" s="176"/>
+      <c r="A16" s="190" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="191"/>
+      <c r="C16" s="191"/>
       <c r="D16" s="150"/>
       <c r="E16" s="151"/>
     </row>
     <row r="17" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A17" s="177" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="174"/>
-      <c r="C17" s="174"/>
+      <c r="A17" s="192" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="189"/>
+      <c r="C17" s="189"/>
       <c r="D17" s="150"/>
       <c r="E17" s="151"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A18" s="178" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="178"/>
-      <c r="C18" s="178"/>
+      <c r="A18" s="193" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="193"/>
+      <c r="C18" s="193"/>
       <c r="D18" s="152"/>
       <c r="E18" s="152"/>
     </row>
     <row r="19" spans="1:5" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A19" s="179" t="s">
+      <c r="A19" s="194" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="180"/>
-      <c r="C19" s="181"/>
+      <c r="B19" s="195"/>
+      <c r="C19" s="196"/>
       <c r="D19" s="155">
         <v>0</v>
       </c>
@@ -3949,20 +4003,20 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="54" customHeight="1">
-      <c r="A22" s="172"/>
-      <c r="B22" s="172"/>
-      <c r="C22" s="172"/>
-      <c r="D22" s="172"/>
-      <c r="E22" s="172"/>
+      <c r="A22" s="181"/>
+      <c r="B22" s="181"/>
+      <c r="C22" s="181"/>
+      <c r="D22" s="181"/>
+      <c r="E22" s="181"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A23" s="173" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="173"/>
-      <c r="C23" s="173"/>
-      <c r="D23" s="173"/>
-      <c r="E23" s="173"/>
+      <c r="A23" s="188" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="188"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="188"/>
     </row>
     <row r="24" spans="1:5" ht="36" customHeight="1">
       <c r="A24" s="1"/>
@@ -3972,13 +4026,14 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1">
-      <c r="A25" s="173" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="173"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
+      <c r="A25" s="188" t="str">
+        <f xml:space="preserve"> CONCATENATE("План розглянуто на засіданні кафедри", 'СПИСКИ (пароль 123)'!J2, 'СПИСКИ (пароль 123)'!J3)</f>
+        <v>План розглянуто на засіданні кафедри" 30 " серпня 2021 р. Протокол № 1</v>
+      </c>
+      <c r="B25" s="188"/>
+      <c r="C25" s="188"/>
+      <c r="D25" s="188"/>
+      <c r="E25" s="188"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
@@ -3989,16 +4044,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C1:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A25:E25"/>
@@ -4007,6 +4052,16 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4022,7 +4077,7 @@
   <dimension ref="A1:BA70"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageBreakPreview" zoomScale="87" zoomScaleNormal="87" zoomScaleSheetLayoutView="87" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="AX2" sqref="AX2:AY3"/>
@@ -4073,7 +4128,7 @@
     <col min="48" max="49" width="4.5703125" style="1" customWidth="1"/>
     <col min="50" max="51" width="5.7109375" style="2" customWidth="1"/>
     <col min="52" max="52" width="11" style="1" customWidth="1"/>
-    <col min="53" max="53" width="11.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="54" max="54" width="11.5703125" style="1" customWidth="1"/>
     <col min="55" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -4134,177 +4189,177 @@
       <c r="AY1" s="136"/>
     </row>
     <row r="2" spans="1:51" s="136" customFormat="1" ht="36" customHeight="1">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="227" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="188" t="s">
+      <c r="B2" s="227" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="202" t="s">
+      <c r="C2" s="233" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="202" t="s">
+      <c r="D2" s="233" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="216" t="s">
+      <c r="E2" s="201" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="218" t="s">
+      <c r="F2" s="203" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="188" t="s">
+      <c r="G2" s="227" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="195" t="s">
+      <c r="H2" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="199"/>
-      <c r="J2" s="195" t="s">
+      <c r="I2" s="207"/>
+      <c r="J2" s="206" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="199"/>
-      <c r="L2" s="219" t="s">
+      <c r="K2" s="207"/>
+      <c r="L2" s="210" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="220"/>
-      <c r="N2" s="219" t="s">
+      <c r="M2" s="211"/>
+      <c r="N2" s="210" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="220"/>
-      <c r="P2" s="195" t="s">
+      <c r="O2" s="211"/>
+      <c r="P2" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="195" t="s">
+      <c r="Q2" s="198"/>
+      <c r="R2" s="206" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="196"/>
-      <c r="T2" s="191" t="s">
+      <c r="S2" s="198"/>
+      <c r="T2" s="216" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="192"/>
-      <c r="V2" s="195" t="s">
+      <c r="U2" s="217"/>
+      <c r="V2" s="206" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="199"/>
-      <c r="X2" s="191" t="s">
+      <c r="W2" s="207"/>
+      <c r="X2" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" s="192"/>
-      <c r="Z2" s="191" t="s">
+      <c r="Y2" s="217"/>
+      <c r="Z2" s="216" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="192"/>
-      <c r="AB2" s="191" t="s">
+      <c r="AA2" s="217"/>
+      <c r="AB2" s="216" t="s">
         <v>54</v>
       </c>
-      <c r="AC2" s="192"/>
-      <c r="AD2" s="223" t="s">
+      <c r="AC2" s="217"/>
+      <c r="AD2" s="220" t="s">
         <v>55</v>
       </c>
-      <c r="AE2" s="224"/>
-      <c r="AF2" s="191" t="s">
+      <c r="AE2" s="221"/>
+      <c r="AF2" s="216" t="s">
         <v>56</v>
       </c>
-      <c r="AG2" s="192"/>
-      <c r="AH2" s="191" t="s">
+      <c r="AG2" s="217"/>
+      <c r="AH2" s="216" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="192"/>
-      <c r="AJ2" s="191" t="s">
+      <c r="AI2" s="217"/>
+      <c r="AJ2" s="216" t="s">
         <v>58</v>
       </c>
-      <c r="AK2" s="192"/>
-      <c r="AL2" s="191" t="s">
+      <c r="AK2" s="217"/>
+      <c r="AL2" s="216" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="192"/>
-      <c r="AN2" s="191" t="s">
+      <c r="AM2" s="217"/>
+      <c r="AN2" s="216" t="s">
         <v>60</v>
       </c>
-      <c r="AO2" s="192"/>
-      <c r="AP2" s="191" t="s">
+      <c r="AO2" s="217"/>
+      <c r="AP2" s="216" t="s">
         <v>61</v>
       </c>
-      <c r="AQ2" s="192"/>
-      <c r="AR2" s="209" t="s">
+      <c r="AQ2" s="217"/>
+      <c r="AR2" s="228" t="s">
         <v>62</v>
       </c>
-      <c r="AS2" s="210"/>
-      <c r="AT2" s="195" t="s">
+      <c r="AS2" s="229"/>
+      <c r="AT2" s="206" t="s">
         <v>63</v>
       </c>
-      <c r="AU2" s="206"/>
-      <c r="AV2" s="208" t="s">
+      <c r="AU2" s="224"/>
+      <c r="AV2" s="226" t="s">
         <v>64</v>
       </c>
-      <c r="AW2" s="192"/>
-      <c r="AX2" s="213" t="s">
+      <c r="AW2" s="217"/>
+      <c r="AX2" s="197" t="s">
         <v>65</v>
       </c>
-      <c r="AY2" s="196"/>
+      <c r="AY2" s="198"/>
     </row>
     <row r="3" spans="1:51" s="136" customFormat="1" ht="119.25" customHeight="1" thickBot="1">
-      <c r="A3" s="189"/>
-      <c r="B3" s="189"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="217"/>
-      <c r="F3" s="189"/>
-      <c r="G3" s="189"/>
-      <c r="H3" s="200"/>
-      <c r="I3" s="201"/>
-      <c r="J3" s="200"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="221"/>
-      <c r="M3" s="222"/>
-      <c r="N3" s="221"/>
-      <c r="O3" s="222"/>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="198"/>
-      <c r="R3" s="197"/>
-      <c r="S3" s="198"/>
-      <c r="T3" s="193"/>
-      <c r="U3" s="194"/>
-      <c r="V3" s="200"/>
-      <c r="W3" s="201"/>
-      <c r="X3" s="205"/>
-      <c r="Y3" s="194"/>
-      <c r="Z3" s="205"/>
-      <c r="AA3" s="194"/>
-      <c r="AB3" s="205"/>
-      <c r="AC3" s="194"/>
-      <c r="AD3" s="225"/>
-      <c r="AE3" s="226"/>
-      <c r="AF3" s="205"/>
-      <c r="AG3" s="194"/>
-      <c r="AH3" s="205"/>
-      <c r="AI3" s="194"/>
-      <c r="AJ3" s="205"/>
-      <c r="AK3" s="194"/>
-      <c r="AL3" s="205"/>
-      <c r="AM3" s="194"/>
-      <c r="AN3" s="205"/>
-      <c r="AO3" s="194"/>
-      <c r="AP3" s="205"/>
-      <c r="AQ3" s="194"/>
-      <c r="AR3" s="211"/>
-      <c r="AS3" s="212"/>
-      <c r="AT3" s="205"/>
-      <c r="AU3" s="207"/>
-      <c r="AV3" s="207"/>
-      <c r="AW3" s="194"/>
-      <c r="AX3" s="214"/>
-      <c r="AY3" s="215"/>
+      <c r="A3" s="204"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="234"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="209"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="212"/>
+      <c r="M3" s="213"/>
+      <c r="N3" s="212"/>
+      <c r="O3" s="213"/>
+      <c r="P3" s="214"/>
+      <c r="Q3" s="215"/>
+      <c r="R3" s="214"/>
+      <c r="S3" s="215"/>
+      <c r="T3" s="232"/>
+      <c r="U3" s="219"/>
+      <c r="V3" s="208"/>
+      <c r="W3" s="209"/>
+      <c r="X3" s="218"/>
+      <c r="Y3" s="219"/>
+      <c r="Z3" s="218"/>
+      <c r="AA3" s="219"/>
+      <c r="AB3" s="218"/>
+      <c r="AC3" s="219"/>
+      <c r="AD3" s="222"/>
+      <c r="AE3" s="223"/>
+      <c r="AF3" s="218"/>
+      <c r="AG3" s="219"/>
+      <c r="AH3" s="218"/>
+      <c r="AI3" s="219"/>
+      <c r="AJ3" s="218"/>
+      <c r="AK3" s="219"/>
+      <c r="AL3" s="218"/>
+      <c r="AM3" s="219"/>
+      <c r="AN3" s="218"/>
+      <c r="AO3" s="219"/>
+      <c r="AP3" s="218"/>
+      <c r="AQ3" s="219"/>
+      <c r="AR3" s="230"/>
+      <c r="AS3" s="231"/>
+      <c r="AT3" s="218"/>
+      <c r="AU3" s="225"/>
+      <c r="AV3" s="225"/>
+      <c r="AW3" s="219"/>
+      <c r="AX3" s="199"/>
+      <c r="AY3" s="200"/>
     </row>
     <row r="4" spans="1:51" s="127" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="190"/>
-      <c r="B4" s="190"/>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
+      <c r="A4" s="205"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="205"/>
+      <c r="G4" s="205"/>
       <c r="H4" s="145" t="s">
         <v>66</v>
       </c>
@@ -7758,6 +7813,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="T2:U3"/>
+    <mergeCell ref="R2:S3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="AN2:AO3"/>
+    <mergeCell ref="AP2:AQ3"/>
+    <mergeCell ref="AT2:AU3"/>
+    <mergeCell ref="AV2:AW3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="AR2:AS3"/>
     <mergeCell ref="AX2:AY3"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
@@ -7774,19 +7842,6 @@
     <mergeCell ref="AH2:AI3"/>
     <mergeCell ref="AJ2:AK3"/>
     <mergeCell ref="AL2:AM3"/>
-    <mergeCell ref="AN2:AO3"/>
-    <mergeCell ref="AP2:AQ3"/>
-    <mergeCell ref="AT2:AU3"/>
-    <mergeCell ref="AV2:AW3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="AR2:AS3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="T2:U3"/>
-    <mergeCell ref="R2:S3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="AX62:AY63 H19:H30 H16:L16 M13:M16 N13:N30 O13:O32 N30:AW30 I17:M30 N60:AW60 H65:AY65 H13:I15 K13:L15 R11:S11 W31:AY35 I33 K31:K36 M31:M35 Q31:S31 K38:K40 M40 P12:S30 I36 M37 Q36:S40 R34:S35 U33:U35 Q33:S33 R32:S32 I38:I40 T34:T40 O34:O40 H41:T60 U36:AY60 T13:AY30 X5:AY12 T11:W12">
@@ -7824,8 +7879,8 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="90" zoomScaleNormal="75" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="75" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7840,12 +7895,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A1" s="227" t="s">
+      <c r="A1" s="236" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="227"/>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
     </row>
     <row r="2" spans="1:9" ht="79.5" thickBot="1">
       <c r="A2" s="88" t="s">
@@ -8036,12 +8091,12 @@
       <c r="I17" s="65"/>
     </row>
     <row r="18" spans="1:9" s="66" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A18" s="231" t="s">
+      <c r="A18" s="240" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="232"/>
-      <c r="C18" s="232"/>
-      <c r="D18" s="233"/>
+      <c r="B18" s="241"/>
+      <c r="C18" s="241"/>
+      <c r="D18" s="242"/>
       <c r="E18" s="82">
         <f>SUM(E3:E17)</f>
         <v>0</v>
@@ -8055,26 +8110,26 @@
       <c r="I18" s="65"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A19" s="236" t="str">
+      <c r="A19" s="245" t="str">
         <f>CONCATENATE("Викладач ______________      Завідувач кафедри  ____________       / ",'НАВЧАЛЬНА РОБОТА'!BA67," /")</f>
         <v>Викладач ______________      Завідувач кафедри  ____________       / Михайло Годлевський /</v>
       </c>
-      <c r="B19" s="237"/>
-      <c r="C19" s="237"/>
-      <c r="D19" s="237"/>
-      <c r="E19" s="237"/>
-      <c r="F19" s="238"/>
+      <c r="B19" s="246"/>
+      <c r="C19" s="246"/>
+      <c r="D19" s="246"/>
+      <c r="E19" s="246"/>
+      <c r="F19" s="247"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A20" s="227" t="s">
+      <c r="A20" s="236" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="227"/>
-      <c r="C20" s="227"/>
-      <c r="D20" s="227"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
     </row>
     <row r="21" spans="1:9" ht="79.5" thickBot="1">
       <c r="A21" s="73" t="s">
@@ -8161,12 +8216,12 @@
       <c r="F29" s="76"/>
     </row>
     <row r="30" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A30" s="231" t="s">
+      <c r="A30" s="240" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="232"/>
-      <c r="C30" s="232"/>
-      <c r="D30" s="234"/>
+      <c r="B30" s="241"/>
+      <c r="C30" s="241"/>
+      <c r="D30" s="243"/>
       <c r="E30" s="82">
         <f>SUM(E22:E29)</f>
         <v>0</v>
@@ -8177,23 +8232,23 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="228" t="str">
+      <c r="A31" s="237" t="str">
         <f>A19</f>
         <v>Викладач ______________      Завідувач кафедри  ____________       / Михайло Годлевський /</v>
       </c>
-      <c r="B31" s="229"/>
-      <c r="C31" s="229"/>
-      <c r="D31" s="229"/>
-      <c r="E31" s="229"/>
-      <c r="F31" s="230"/>
+      <c r="B31" s="238"/>
+      <c r="C31" s="238"/>
+      <c r="D31" s="238"/>
+      <c r="E31" s="238"/>
+      <c r="F31" s="239"/>
     </row>
     <row r="32" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A32" s="227" t="s">
+      <c r="A32" s="236" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="227"/>
-      <c r="C32" s="227"/>
-      <c r="D32" s="227"/>
+      <c r="B32" s="236"/>
+      <c r="C32" s="236"/>
+      <c r="D32" s="236"/>
     </row>
     <row r="33" spans="1:6" ht="48" thickBot="1">
       <c r="A33" s="77" t="s">
@@ -8256,12 +8311,12 @@
       <c r="F38" s="67"/>
     </row>
     <row r="39" spans="1:6" s="66" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A39" s="235" t="s">
+      <c r="A39" s="244" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="232"/>
-      <c r="C39" s="232"/>
-      <c r="D39" s="234"/>
+      <c r="B39" s="241"/>
+      <c r="C39" s="241"/>
+      <c r="D39" s="243"/>
       <c r="E39" s="82">
         <f>SUM(E34:E38)</f>
         <v>0</v>
@@ -8272,15 +8327,15 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A40" s="228" t="str">
+      <c r="A40" s="237" t="str">
         <f>A31</f>
         <v>Викладач ______________      Завідувач кафедри  ____________       / Михайло Годлевський /</v>
       </c>
-      <c r="B40" s="229"/>
-      <c r="C40" s="229"/>
-      <c r="D40" s="229"/>
-      <c r="E40" s="229"/>
-      <c r="F40" s="230"/>
+      <c r="B40" s="238"/>
+      <c r="C40" s="238"/>
+      <c r="D40" s="238"/>
+      <c r="E40" s="238"/>
+      <c r="F40" s="239"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1"/>
@@ -8319,8 +8374,8 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8338,14 +8393,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="227" t="s">
+      <c r="A1" s="236" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="227"/>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
       <c r="G1" s="143"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -8467,182 +8522,187 @@
       <c r="G9" s="32"/>
     </row>
     <row r="11" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A11" s="241" t="s">
+      <c r="A11" s="249" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="241"/>
-      <c r="C11" s="241"/>
-      <c r="D11" s="241"/>
-      <c r="E11" s="241"/>
-      <c r="F11" s="241"/>
-      <c r="G11" s="241"/>
+      <c r="B11" s="249"/>
+      <c r="C11" s="249"/>
+      <c r="D11" s="249"/>
+      <c r="E11" s="249"/>
+      <c r="F11" s="249"/>
+      <c r="G11" s="249"/>
     </row>
     <row r="12" spans="1:11" ht="51" thickBot="1">
       <c r="A12" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="242" t="s">
+      <c r="B12" s="250" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="242"/>
-      <c r="D12" s="242"/>
-      <c r="E12" s="242"/>
-      <c r="F12" s="242"/>
+      <c r="C12" s="250"/>
+      <c r="D12" s="250"/>
+      <c r="E12" s="250"/>
+      <c r="F12" s="250"/>
       <c r="G12" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="52.5" customHeight="1">
       <c r="A13" s="18"/>
-      <c r="B13" s="243" t="e">
-        <f>CONCATENATE("Звіт про виконання індивідуального плану за ",ТИТУЛ!A34," навчальний рік викладача ",ТИТУЛ!A24," розглянуто ___  _____________ 20__ р. на засіданні кафедри ",ТИТУЛ!B12," й ухвалено рішення (протокол №______): Індивідуальний план виконано в обсязі ",#REF!," годин.")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C13" s="244"/>
-      <c r="D13" s="244"/>
-      <c r="E13" s="244"/>
-      <c r="F13" s="245"/>
+      <c r="B13" s="251" t="str">
+        <f>CONCATENATE("Звіт про виконання індивідуального плану за ",ТИТУЛ!A34," навчальний рік викладача ", ТИТУЛ!A24," розглянуто ", 'СПИСКИ (пароль 123)'!J2," на засіданні кафедри ", ТИТУЛ!B12," й ухвалено рішення (",'СПИСКИ (пароль 123)'!J3,"): Індивідуальний план виконано в повному обсязі. ")</f>
+        <v xml:space="preserve">Звіт про виконання індивідуального плану за 2020 / 2021 навчальний рік викладача Викладач 14 розглянуто " 30 " серпня 2021 р.  на засіданні кафедри Програмної інженерії та інформаційних технологій управління й ухвалено рішення (Протокол № 1): Індивідуальний план виконано в повному обсязі. </v>
+      </c>
+      <c r="C13" s="252"/>
+      <c r="D13" s="252"/>
+      <c r="E13" s="252"/>
+      <c r="F13" s="253"/>
       <c r="G13" s="24"/>
     </row>
     <row r="14" spans="1:11" ht="44.25" customHeight="1">
       <c r="A14" s="19"/>
-      <c r="B14" s="246" t="s">
+      <c r="B14" s="254" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="247"/>
-      <c r="D14" s="247"/>
-      <c r="E14" s="247"/>
-      <c r="F14" s="248"/>
+      <c r="C14" s="255"/>
+      <c r="D14" s="255"/>
+      <c r="E14" s="255"/>
+      <c r="F14" s="256"/>
       <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:11" ht="32.25" customHeight="1">
       <c r="A15" s="19"/>
-      <c r="B15" s="239"/>
-      <c r="C15" s="239"/>
-      <c r="D15" s="239"/>
-      <c r="E15" s="239"/>
-      <c r="F15" s="239"/>
+      <c r="B15" s="248"/>
+      <c r="C15" s="248"/>
+      <c r="D15" s="248"/>
+      <c r="E15" s="248"/>
+      <c r="F15" s="248"/>
       <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:11" ht="32.25" customHeight="1">
       <c r="A16" s="19"/>
-      <c r="B16" s="239"/>
-      <c r="C16" s="239"/>
-      <c r="D16" s="239"/>
-      <c r="E16" s="239"/>
-      <c r="F16" s="239"/>
+      <c r="B16" s="248"/>
+      <c r="C16" s="248"/>
+      <c r="D16" s="248"/>
+      <c r="E16" s="248"/>
+      <c r="F16" s="248"/>
       <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1">
       <c r="A17" s="19"/>
-      <c r="B17" s="239"/>
-      <c r="C17" s="239"/>
-      <c r="D17" s="239"/>
-      <c r="E17" s="239"/>
-      <c r="F17" s="239"/>
+      <c r="B17" s="248"/>
+      <c r="C17" s="248"/>
+      <c r="D17" s="248"/>
+      <c r="E17" s="248"/>
+      <c r="F17" s="248"/>
       <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" ht="32.25" customHeight="1" thickBot="1">
       <c r="A18" s="20"/>
-      <c r="B18" s="240"/>
-      <c r="C18" s="240"/>
-      <c r="D18" s="240"/>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
+      <c r="B18" s="257"/>
+      <c r="C18" s="257"/>
+      <c r="D18" s="257"/>
+      <c r="E18" s="257"/>
+      <c r="F18" s="257"/>
       <c r="G18" s="32"/>
     </row>
     <row r="20" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A20" s="241" t="s">
+      <c r="A20" s="249" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="241"/>
-      <c r="C20" s="241"/>
-      <c r="D20" s="241"/>
-      <c r="E20" s="241"/>
-      <c r="F20" s="241"/>
-      <c r="G20" s="241"/>
+      <c r="B20" s="249"/>
+      <c r="C20" s="249"/>
+      <c r="D20" s="249"/>
+      <c r="E20" s="249"/>
+      <c r="F20" s="249"/>
+      <c r="G20" s="249"/>
     </row>
     <row r="21" spans="1:7" ht="30" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="242" t="s">
+      <c r="B21" s="250" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="242"/>
-      <c r="D21" s="242"/>
-      <c r="E21" s="242"/>
-      <c r="F21" s="242"/>
+      <c r="C21" s="250"/>
+      <c r="D21" s="250"/>
+      <c r="E21" s="250"/>
+      <c r="F21" s="250"/>
       <c r="G21" s="14" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="32.25" customHeight="1">
       <c r="A22" s="18"/>
-      <c r="B22" s="249"/>
-      <c r="C22" s="249"/>
-      <c r="D22" s="249"/>
-      <c r="E22" s="249"/>
-      <c r="F22" s="249"/>
+      <c r="B22" s="258"/>
+      <c r="C22" s="258"/>
+      <c r="D22" s="258"/>
+      <c r="E22" s="258"/>
+      <c r="F22" s="258"/>
       <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:7" ht="32.25" customHeight="1">
       <c r="A23" s="19"/>
-      <c r="B23" s="239"/>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
+      <c r="B23" s="248"/>
+      <c r="C23" s="248"/>
+      <c r="D23" s="248"/>
+      <c r="E23" s="248"/>
+      <c r="F23" s="248"/>
       <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="32.25" customHeight="1">
       <c r="A24" s="19"/>
-      <c r="B24" s="239"/>
-      <c r="C24" s="239"/>
-      <c r="D24" s="239"/>
-      <c r="E24" s="239"/>
-      <c r="F24" s="239"/>
+      <c r="B24" s="248"/>
+      <c r="C24" s="248"/>
+      <c r="D24" s="248"/>
+      <c r="E24" s="248"/>
+      <c r="F24" s="248"/>
       <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" ht="32.25" customHeight="1">
       <c r="A25" s="19"/>
-      <c r="B25" s="239"/>
-      <c r="C25" s="239"/>
-      <c r="D25" s="239"/>
-      <c r="E25" s="239"/>
-      <c r="F25" s="239"/>
+      <c r="B25" s="248"/>
+      <c r="C25" s="248"/>
+      <c r="D25" s="248"/>
+      <c r="E25" s="248"/>
+      <c r="F25" s="248"/>
       <c r="G25" s="28"/>
     </row>
     <row r="26" spans="1:7" ht="32.25" customHeight="1">
       <c r="A26" s="19"/>
-      <c r="B26" s="239"/>
-      <c r="C26" s="239"/>
-      <c r="D26" s="239"/>
-      <c r="E26" s="239"/>
-      <c r="F26" s="239"/>
+      <c r="B26" s="248"/>
+      <c r="C26" s="248"/>
+      <c r="D26" s="248"/>
+      <c r="E26" s="248"/>
+      <c r="F26" s="248"/>
       <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" ht="32.25" customHeight="1">
       <c r="A27" s="19"/>
-      <c r="B27" s="239"/>
-      <c r="C27" s="239"/>
-      <c r="D27" s="239"/>
-      <c r="E27" s="239"/>
-      <c r="F27" s="239"/>
+      <c r="B27" s="248"/>
+      <c r="C27" s="248"/>
+      <c r="D27" s="248"/>
+      <c r="E27" s="248"/>
+      <c r="F27" s="248"/>
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="32.25" customHeight="1" thickBot="1">
       <c r="A28" s="20"/>
-      <c r="B28" s="240"/>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="240"/>
-      <c r="F28" s="240"/>
+      <c r="B28" s="257"/>
+      <c r="C28" s="257"/>
+      <c r="D28" s="257"/>
+      <c r="E28" s="257"/>
+      <c r="F28" s="257"/>
       <c r="G28" s="32"/>
     </row>
   </sheetData>
   <sheetProtection password="CA9C" sheet="1" formatCells="0" selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="A1:F1"/>
@@ -8656,11 +8716,6 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -8672,10 +8727,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -8689,9 +8744,10 @@
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" style="44" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" customHeight="1">
+    <row r="1" spans="1:10" ht="21" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>94</v>
       </c>
@@ -8719,8 +8775,11 @@
       <c r="I1" s="44" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1">
+      <c r="J1" s="157" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1">
       <c r="A2" s="33"/>
       <c r="E2" s="33"/>
       <c r="G2" s="33"/>
@@ -8728,8 +8787,11 @@
       <c r="I2" s="44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="22.5" customHeight="1">
+      <c r="J2" s="158" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="22.5" customHeight="1">
       <c r="A3" s="45" t="s">
         <v>8</v>
       </c>
@@ -8757,8 +8819,11 @@
       <c r="I3" s="45" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="22.5" customHeight="1">
+      <c r="J3" s="159" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="22.5" customHeight="1">
       <c r="A4" s="45"/>
       <c r="B4" s="43"/>
       <c r="C4" s="45"/>
@@ -8774,8 +8839,9 @@
       <c r="I4" s="45" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="22.5" customHeight="1">
+      <c r="J4" s="156"/>
+    </row>
+    <row r="5" spans="1:10" ht="22.5" customHeight="1">
       <c r="A5" s="45"/>
       <c r="B5" s="43"/>
       <c r="C5" s="45"/>
@@ -8789,7 +8855,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="22.5" customHeight="1">
+    <row r="6" spans="1:10" ht="22.5" customHeight="1">
       <c r="A6" s="45"/>
       <c r="B6" s="43"/>
       <c r="C6" s="45"/>
@@ -8803,7 +8869,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.5" customHeight="1">
+    <row r="7" spans="1:10" ht="22.5" customHeight="1">
       <c r="A7" s="45"/>
       <c r="B7" s="43"/>
       <c r="C7" s="45"/>
@@ -8815,7 +8881,7 @@
       </c>
       <c r="H7" s="33"/>
     </row>
-    <row r="8" spans="1:9" ht="22.5" customHeight="1">
+    <row r="8" spans="1:10" ht="22.5" customHeight="1">
       <c r="A8" s="45"/>
       <c r="B8" s="43"/>
       <c r="C8" s="45"/>
@@ -8825,7 +8891,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="33"/>
     </row>
-    <row r="9" spans="1:9" ht="22.5" customHeight="1">
+    <row r="9" spans="1:10" ht="22.5" customHeight="1">
       <c r="A9" s="45"/>
       <c r="B9" s="43"/>
       <c r="C9" s="45"/>
@@ -8835,7 +8901,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="33"/>
     </row>
-    <row r="10" spans="1:9" ht="22.5" customHeight="1">
+    <row r="10" spans="1:10" ht="22.5" customHeight="1">
       <c r="A10" s="33"/>
       <c r="D10" s="46"/>
       <c r="E10" s="45"/>
@@ -8843,7 +8909,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="33"/>
     </row>
-    <row r="11" spans="1:9" ht="22.5" customHeight="1">
+    <row r="11" spans="1:10" ht="22.5" customHeight="1">
       <c r="A11" s="33"/>
       <c r="D11" s="46"/>
       <c r="E11" s="45"/>
@@ -8851,7 +8917,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="33"/>
     </row>
-    <row r="12" spans="1:9" ht="22.5" customHeight="1">
+    <row r="12" spans="1:10" ht="22.5" customHeight="1">
       <c r="A12" s="33"/>
       <c r="D12" s="46"/>
       <c r="E12" s="45"/>
@@ -8859,7 +8925,7 @@
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
     </row>
-    <row r="13" spans="1:9" ht="22.5" customHeight="1">
+    <row r="13" spans="1:10" ht="22.5" customHeight="1">
       <c r="A13" s="33"/>
       <c r="D13" s="46"/>
       <c r="E13" s="45"/>
@@ -8867,7 +8933,7 @@
       <c r="G13" s="33"/>
       <c r="H13" s="33"/>
     </row>
-    <row r="14" spans="1:9" ht="22.5" customHeight="1">
+    <row r="14" spans="1:10" ht="22.5" customHeight="1">
       <c r="A14" s="33"/>
       <c r="D14" s="46"/>
       <c r="E14" s="45"/>
@@ -8875,7 +8941,7 @@
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
     </row>
-    <row r="15" spans="1:9" ht="22.5" customHeight="1">
+    <row r="15" spans="1:10" ht="22.5" customHeight="1">
       <c r="A15" s="33"/>
       <c r="D15" s="46"/>
       <c r="E15" s="45"/>
@@ -8883,7 +8949,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="22.5" customHeight="1">
+    <row r="16" spans="1:10" ht="22.5" customHeight="1">
       <c r="A16" s="33"/>
       <c r="D16" s="46"/>
       <c r="E16" s="45"/>

</xml_diff>

<commit_message>
almost final version, zmini_ta_visnovki shit
</commit_message>
<xml_diff>
--- a/IndPlanExample.xlsx
+++ b/IndPlanExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Trash\IntelliJ IDEA 2020.3.2\workspace\SLDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B80D69-F6B2-43D2-8FA8-D56BCBA1247F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60B4C2-35AB-427B-A7A6-A5E356AE0EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="926" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="926" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТИТУЛ" sheetId="1" r:id="rId1"/>
@@ -8374,8 +8374,8 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8549,10 +8549,7 @@
     </row>
     <row r="13" spans="1:11" ht="52.5" customHeight="1">
       <c r="A13" s="18"/>
-      <c r="B13" s="251" t="str">
-        <f>CONCATENATE("Звіт про виконання індивідуального плану за ",ТИТУЛ!A34," навчальний рік викладача ", ТИТУЛ!A24," розглянуто ", 'СПИСКИ (пароль 123)'!J2," на засіданні кафедри ", ТИТУЛ!B12," й ухвалено рішення (",'СПИСКИ (пароль 123)'!J3,"): Індивідуальний план виконано в повному обсязі. ")</f>
-        <v xml:space="preserve">Звіт про виконання індивідуального плану за 2020 / 2021 навчальний рік викладача Викладач 14 розглянуто " 30 " серпня 2021 р.  на засіданні кафедри Програмної інженерії та інформаційних технологій управління й ухвалено рішення (Протокол № 1): Індивідуальний план виконано в повному обсязі. </v>
-      </c>
+      <c r="B13" s="251"/>
       <c r="C13" s="252"/>
       <c r="D13" s="252"/>
       <c r="E13" s="252"/>

</xml_diff>